<commit_message>
Code Update with implementing HEM (include doublecounting) and first attempts of a new approach to make out contribution of upstream product groups to final demand
</commit_message>
<xml_diff>
--- a/Y_2002_ImpNoExpNoCII_Base.xlsx
+++ b/Y_2002_ImpNoExpNoCII_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jstreeck\Desktop\EndUse_shortTermSave\2020_NationalOfficial_IOSUT\USA\Benchmark_SUTIO\_NewResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED92926-3E20-4C98-8EC3-A104B1CF1BD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88422C49-0DAA-4F06-9F6A-7C44D1DDD34C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2605,10 +2605,10 @@
     <t>commodity_ID</t>
   </si>
   <si>
-    <t>commidity_label</t>
-  </si>
-  <si>
     <t>final_demand</t>
+  </si>
+  <si>
+    <t>commodity_label</t>
   </si>
 </sst>
 </file>
@@ -3013,26 +3013,26 @@
   <dimension ref="A1:C431"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>860</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>861</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>656.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>13850.8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>839.7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>9666.7000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>12831.2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>207.2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>81.400000000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>2686.2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>2653.1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>2421.5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>415.8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>46.3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>63.3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>41.1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>13238.8</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>107106.1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>38490</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>25711.200000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>129239.3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>23465.599999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>292328.09999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>304950.8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>129170</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>9080.2999999999993</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>1604.7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>1639.1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>220.9</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>2848</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>309.2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>7262.7</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>1236.4000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>952.2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>9250.6</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>6619.9</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>16928.599999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>20118.2</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>8882.1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>4607</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>15494.3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>2411.9</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>22906.5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>42571.6</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>3517.8</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>32074.7</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>13627.9</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>1323.4</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>15134</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>3446.5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>63.1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>6762.7</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>11210.1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>28327.4</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>22202.1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>10209.9</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>6843.4</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>43319.9</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>132.80000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>991.2</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>165.6</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>157.80000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>499.4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>11861.7</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>11122</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>881.5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>2733</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>3640.6</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>34185.1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>52371.5</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>5195</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>4045.9</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>17191.2</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>5137.8</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>6907.3</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>1985.4</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>10345.5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>521.79999999999995</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>1254.5999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>79.900000000000006</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>797.9</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>4544.5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>894.3</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>2185.3000000000002</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>65954.399999999994</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>2014.9</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>221.6</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>127.6</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>2522.8000000000002</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>577.20000000000005</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>116.1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>3037.1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>131</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>107741.6</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>134</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>135</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>415.6</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>136</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>688.8</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>17265.900000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>28007.5</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>139</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>140</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>2276.5</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>2460.5</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>437.4</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>464.1</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>7462.9</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>6912.3</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>150</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>315.7</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>151</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>970.6</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>2314.1</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>153</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>154</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>155</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>2721.1</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>157</v>
       </c>
@@ -4770,7 +4770,7 @@
         <v>159.69999999999999</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>158</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>722.2</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>159</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>160</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>161</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>163</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>164</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>133.1</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>165</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>1653.6</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>166</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>114.5</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>167</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>168</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>169</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>170</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>580.9</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>171</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>172</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>173</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>174</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>175</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>176</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>177</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>178</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>179</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>180</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>181</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>182</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>312.3</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>183</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>3180.3</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>184</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>1979.1</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>185</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>190.3</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>186</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>335.1</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>187</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>1316.4</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>188</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>189</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>331.9</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>190</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>511.5</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>191</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>82.6</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>192</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>884.2</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>193</v>
       </c>
@@ -5166,7 +5166,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>194</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>195</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>196</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>197</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>198</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>431.7</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>199</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>757.9</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>200</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>2750.9</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>201</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>2296.5</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>202</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>12799.3</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>203</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>5655.4000000000005</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>204</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>15466.4</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>205</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>1992.6</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>206</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>2722.1</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>207</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>7038.4</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>208</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>14602.1</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>209</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>1452.5</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>210</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>3596.3</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>211</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>7949.6</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>212</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>4806.2</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>213</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>214</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>6539.8</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>215</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>2127.9</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>216</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>5708.5</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>217</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>7111.8</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>218</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>219</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>4067.3</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>220</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>2809.5</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>221</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>10040.799999999999</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>222</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>223</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>224</v>
       </c>
@@ -5507,7 +5507,7 @@
         <v>2293</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>225</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>5131.8999999999996</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>226</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>3367.2</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>227</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>11269.7</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>228</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>4503.2</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>229</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>3616.4</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>230</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>776.6</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>231</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>7546.2999999999993</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>232</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>285.8</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>233</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>46989.7</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>234</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>6093.1</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>235</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>25737.4</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>236</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>24619.9</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>237</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>32849</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>238</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>1088.7</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>239</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>33961.199999999997</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>240</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>241</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>242</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>243</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>244</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>405.4</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>245</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>568.40000000000009</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>246</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>247</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>13566.1</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>248</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>20640.400000000001</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>249</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>250</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>4120.0999999999995</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>251</v>
       </c>
@@ -5804,7 +5804,7 @@
         <v>1687.9</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>252</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>5697.5</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>253</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>5530.3</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>254</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>4311.9000000000005</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>255</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>5874.9</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>256</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>727.5</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>257</v>
       </c>
@@ -5870,7 +5870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>258</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>1123.9000000000001</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>259</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>2909.8</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>260</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>8016</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>261</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>6225.8</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>262</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>5645.7999999999993</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>263</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>4098.5</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>264</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>2023.6</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>265</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>3767.2</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>266</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>267</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>3268.5</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>268</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>1618.3</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>269</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>270</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>2595.6</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>271</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>343.4</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>272</v>
       </c>
@@ -6035,7 +6035,7 @@
         <v>283.89999999999998</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>273</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>274</v>
       </c>
@@ -6057,7 +6057,7 @@
         <v>5784.0000000000009</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>275</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>132930.79999999999</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>276</v>
       </c>
@@ -6079,7 +6079,7 @@
         <v>184044.9</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>277</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>18523.900000000001</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>278</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>1921.7</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>279</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>3865.8</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>280</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>4961.2</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>281</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>5304.9000000000005</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>282</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>10693.8</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>283</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>34935.199999999997</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>284</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>1227.3</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>285</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>286</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>4457.6000000000004</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>287</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>1334.3</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>288</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>4812.5999999999995</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>289</v>
       </c>
@@ -6222,7 +6222,7 @@
         <v>9044.3000000000011</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>290</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>7982.0000000000009</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>291</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>6506.2000000000007</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>292</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>1281.2</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>293</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>5831</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>294</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>1547.9</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>295</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>11734.3</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>296</v>
       </c>
@@ -6299,7 +6299,7 @@
         <v>17946</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>297</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>5442.9</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>298</v>
       </c>
@@ -6321,7 +6321,7 @@
         <v>4408.8</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>299</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>11701.2</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>300</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>6879.1</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>301</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>58.7</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>302</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>4888.5</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>303</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>3100.8</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>304</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>4435.8</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>305</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>13620.8</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>306</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>9127.1999999999989</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>307</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>1083.3</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>308</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>5731.7</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>309</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>310</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>23034.2</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>311</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>14559.5</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>312</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>17827.400000000001</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>313</v>
       </c>
@@ -6486,7 +6486,7 @@
         <v>2066.6999999999998</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>314</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>6189.7</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>315</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>142.69999999999999</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>316</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>2585.6</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>317</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>1343.6</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>318</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>13739.8</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>319</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>399965.6</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>320</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>68076.399999999994</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>321</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>6323.1999999999989</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>322</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>8539.7000000000007</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>323</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>73044.999999999985</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>324</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>20957.599999999999</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>325</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>1324.8</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>326</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>3434.6</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>327</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>7913.8</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>328</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>1345.2</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>329</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>291.5</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>330</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>826595.70000000007</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>331</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>13797.2</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>332</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>12947.6</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>333</v>
       </c>
@@ -6706,7 +6706,7 @@
         <v>20525.7</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>334</v>
       </c>
@@ -6717,7 +6717,7 @@
         <v>6824.2</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>335</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>67278.399999999994</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>336</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>25448.400000000001</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>337</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>10290.9</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>338</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>2463.3000000000002</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>339</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>340</v>
       </c>
@@ -6783,7 +6783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>341</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>193096.6</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>342</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>21929</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>343</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>344</v>
       </c>
@@ -6827,7 +6827,7 @@
         <v>3073</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>345</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>24951.200000000001</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>346</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>100820.9</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>347</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>205599.6</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>348</v>
       </c>
@@ -6871,7 +6871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>349</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>80244</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>350</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>154152.79999999999</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>351</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>324552.3</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>352</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>42097.2</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>353</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>7995.9</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>354</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>76.8</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>355</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>16708.2</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>356</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>357</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>75810</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>358</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>12497.6</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>359</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>28849.5</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>360</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>1701.6</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>361</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>140560.6</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>362</v>
       </c>
@@ -7025,7 +7025,7 @@
         <v>11531</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>363</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>364</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>365</v>
       </c>
@@ -7058,7 +7058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>366</v>
       </c>
@@ -7069,7 +7069,7 @@
         <v>10588.3</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>367</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>959.7</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>368</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>6630.4</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>369</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>12266.8</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>370</v>
       </c>
@@ -7113,7 +7113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>371</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>372</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>373</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>374</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>661.9</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>375</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>4345.1000000000004</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>376</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>8976.2999999999993</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>377</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>6820.6</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>378</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>7845.9</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>379</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>537.9</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>380</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>11010.2</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>381</v>
       </c>
@@ -7234,7 +7234,7 @@
         <v>32224.6</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>382</v>
       </c>
@@ -7245,7 +7245,7 @@
         <v>108487.8</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
         <v>383</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>35423</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>384</v>
       </c>
@@ -7267,7 +7267,7 @@
         <v>47346.7</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
         <v>385</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>380223.5</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>386</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>97267.7</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>387</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>470477.7</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>388</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>131542.29999999999</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>389</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>22832.799999999999</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>390</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>34463.300000000003</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>391</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>43525.7</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>392</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>8657</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>393</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>11470.2</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>394</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>94.9</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>395</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>8568.6</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>396</v>
       </c>
@@ -7399,7 +7399,7 @@
         <v>8187.7</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>397</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>12190.5</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>398</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>2284.4</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>399</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>66374.899999999994</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>400</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>20926.5</v>
       </c>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>401</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>43829.599999999999</v>
       </c>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>402</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>17763.8</v>
       </c>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>403</v>
       </c>
@@ -7476,7 +7476,7 @@
         <v>370904.7</v>
       </c>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>404</v>
       </c>
@@ -7487,7 +7487,7 @@
         <v>6726.4</v>
       </c>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>405</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>129304.3</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>406</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>3974.9</v>
       </c>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>407</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>408</v>
       </c>
@@ -7531,7 +7531,7 @@
         <v>14435.4</v>
       </c>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>409</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>38222.400000000001</v>
       </c>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>410</v>
       </c>
@@ -7553,7 +7553,7 @@
         <v>13953.3</v>
       </c>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>411</v>
       </c>
@@ -7564,7 +7564,7 @@
         <v>13047</v>
       </c>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>412</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>46952.2</v>
       </c>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>413</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>64380.4</v>
       </c>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>414</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>27469.599999999999</v>
       </c>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>415</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>30816.2</v>
       </c>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>416</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>12515.5</v>
       </c>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>417</v>
       </c>
@@ -7630,7 +7630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
         <v>418</v>
       </c>
@@ -7641,7 +7641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
         <v>419</v>
       </c>
@@ -7652,7 +7652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
         <v>420</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
         <v>421</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>39860.199999999997</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
         <v>422</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>55944.2</v>
       </c>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
         <v>423</v>
       </c>
@@ -7696,7 +7696,7 @@
         <v>-7470.7999999999993</v>
       </c>
     </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
         <v>424</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>-6873.9</v>
       </c>
     </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
         <v>425</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>380796.9</v>
       </c>
     </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
         <v>426</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>209856</v>
       </c>
     </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
         <v>427</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>1042157.4</v>
       </c>
     </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
         <v>428</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>959446</v>
       </c>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
         <v>429</v>
       </c>

</xml_diff>